<commit_message>
Mudar imagens e texto
</commit_message>
<xml_diff>
--- a/db/Produtos.xlsx
+++ b/db/Produtos.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21514"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo Coto\PycharmProjects\Loja0321\db\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F40585-FEAD-4E02-B860-2F0C6D0428EF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5952" yWindow="4008" windowWidth="23040" windowHeight="12204" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5955" yWindow="4005" windowWidth="19440" windowHeight="12210"/>
   </bookViews>
   <sheets>
-    <sheet name="Monitores" sheetId="2" r:id="rId1"/>
+    <sheet name="Cães" sheetId="2" r:id="rId1"/>
     <sheet name="Placas Gráficas" sheetId="1" r:id="rId2"/>
     <sheet name="Caixas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="74">
   <si>
     <t>Código</t>
   </si>
@@ -145,33 +139,12 @@
     <t>RX 590</t>
   </si>
   <si>
-    <t>Tamanho</t>
-  </si>
-  <si>
-    <t>Sync</t>
-  </si>
-  <si>
     <t>Asus</t>
   </si>
   <si>
     <t>AOC</t>
   </si>
   <si>
-    <t>Acer</t>
-  </si>
-  <si>
-    <t>BenQ</t>
-  </si>
-  <si>
-    <t>Dell</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>LG</t>
-  </si>
-  <si>
     <t>Sku</t>
   </si>
   <si>
@@ -245,12 +218,39 @@
   </si>
   <si>
     <t>18</t>
+  </si>
+  <si>
+    <t>ROYAL CANIN BABYDOG MILK</t>
+  </si>
+  <si>
+    <t>ROYAL CANIN GIANT ADULT</t>
+  </si>
+  <si>
+    <t>DELI BAKIE STARS</t>
+  </si>
+  <si>
+    <t>Proplan Dental Probar 150gr</t>
+  </si>
+  <si>
+    <t>NERF TEETHER FOOTBALL</t>
+  </si>
+  <si>
+    <t>NERF TIRE SQUEAK FOOTBALL</t>
+  </si>
+  <si>
+    <t>BOLAS DE TÉNIS</t>
+  </si>
+  <si>
+    <t>NERF TIRE INFINITY TUG</t>
+  </si>
+  <si>
+    <t>JAULA TRANSPORTADORA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
@@ -310,13 +310,7 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom"/>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <alignment horizontal="center" vertical="bottom"/>
     </dxf>
@@ -346,29 +340,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela13" displayName="Tabela13" ref="A1:E13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Código" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Marca" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tamanho" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sync" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Preço" dataDxfId="0" dataCellStyle="Moeda"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela13" displayName="Tabela13" ref="A1:C13" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C13"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Código" dataDxfId="2"/>
+    <tableColumn id="2" name="Nome" dataDxfId="1"/>
+    <tableColumn id="3" name="Preço" dataDxfId="0" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela1" displayName="Tabela1" ref="A1:F13" totalsRowShown="0">
-  <autoFilter ref="A1:F13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F13" totalsRowShown="0">
+  <autoFilter ref="A1:F13"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Código"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Fabricante"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Marca"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Designação"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Quantidade"/>
-    <tableColumn id="6" xr3:uid="{FFB35986-AE7C-4950-9091-2B68C9ECF840}" name="Preço" dataCellStyle="Moeda"/>
+    <tableColumn id="1" name="Código"/>
+    <tableColumn id="3" name="Fabricante"/>
+    <tableColumn id="4" name="Marca"/>
+    <tableColumn id="5" name="Designação"/>
+    <tableColumn id="7" name="Quantidade"/>
+    <tableColumn id="6" name="Preço" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -417,7 +409,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -450,26 +442,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -502,23 +477,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -694,239 +652,160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F19" sqref="F18:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="5">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="C2" s="5">
+        <v>21.87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="2">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="5">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="C3" s="5">
+        <v>54.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="2">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="2">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="2">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="C6" s="5">
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="5">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="C7" s="5">
+        <v>17.920000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="2">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="5">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="2">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="5">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="C9" s="5">
+        <v>19.329999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="2">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="5">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="C10" s="5">
+        <v>25.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="2">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="5">
+        <v>38</v>
+      </c>
+      <c r="C11" s="5">
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="5">
+        <v>38</v>
+      </c>
+      <c r="C12" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="2">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="5">
+        <v>39</v>
+      </c>
+      <c r="C13" s="5">
         <v>230</v>
       </c>
     </row>
@@ -939,24 +818,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -976,7 +855,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -996,7 +875,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1016,7 +895,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +915,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1056,7 +935,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1076,7 +955,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +975,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1116,7 +995,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1136,7 +1015,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1156,7 +1035,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1176,7 +1055,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1196,7 +1075,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -1225,224 +1104,224 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C2" s="6">
         <v>94.99</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C3" s="6">
         <v>102.99</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6">
         <v>37.99</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C5" s="6">
         <v>23.09</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C6" s="6">
         <v>419.99</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6">
         <v>94.99</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C8" s="6">
         <v>21.19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C9" s="6">
         <v>391.99</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C10" s="6">
         <v>350.99</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C11" s="6">
         <v>267.99</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C12" s="6">
         <v>115.99</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C13" s="6">
         <v>59.99</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C14" s="6">
         <v>69.989999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C15" s="6">
         <v>78.989999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C16" s="6">
         <v>37.79</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C17" s="6">
         <v>51.99</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C18" s="6">
         <v>37.19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C19" s="6">
         <v>19.09</v>

</xml_diff>